<commit_message>
UPDATE: Q&A LLM Fine-Tuning test dataset
</commit_message>
<xml_diff>
--- a/2025_07_02_OhLoRA_ML_Tutor/ai_qna/fine_tuning_dataset/SFT_final.xlsx
+++ b/2025_07_02_OhLoRA_ML_Tutor/ai_qna/fine_tuning_dataset/SFT_final.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904C3FAD-6188-4654-969F-21B8077F2ED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BCE9FC5-7180-45F1-96A6-5F389FE978FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18816" xr2:uid="{E04B2FB7-CC05-43DA-BC72-AD18C1DECBDA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="441">
   <si>
     <t>data_type</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2681,6 +2681,251 @@
   </si>
   <si>
     <t>LLM이 정확히 뭐야? 나도 AI 트렌드 따라잡자!!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>알맞은 정보를 찾을 수 없음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lightGBM? 그게 뭐야?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>XGBoost 가 뭔지 궁금해</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPT-4 알고리즘 자세히 알려줘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DeepSeek 에서 요즘 나온 모델 뭐야?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LLaMA3 언어모델 알고리즘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CNN에서 어떤 Padding 이 쓰이지?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>딥러닝에서 학습률 스케줄러 알려줘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Loss Function 잘못 쓰는 경우 알려줘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LLM 에서 환각 현상이 뭐야?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AGI 는 언제쯤 등장할까?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">XGBoost? 이게 뭐였더라? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😥</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> WannaBeSuperteur 깃헙 계정의 AI-study 레포에 아마 있을 거야!</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">미안 ㅠㅠ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😥</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 나는 인공지능이랑 머신러닝 기초적인 내용만 가지고 있어 ㅠㅠ 그런 건 WannaBeSuperteur 깃헙 계정의 AI-study 레포에서 찾아보면 될 것 같아!</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">GPT-4? GPT가 어떤 알고리즘인지는 WannaBeSuperteur 깃헙 계정의 AI-study 레포 보면 돼! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">DeepSeek? 최신 언어모델 만드는 스타트업 맞지? 아마 WannaBeSuperteur 깃헙 계정의 AI-study 레포 보면 알 수 있을 거야 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이거 최신 언어모델일 텐데? WannaBeSuperteur 깃헙 계정의 AI-study 레포 참고해 봐!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">나는 CNN만 알지 Padding 까지는 자세히는 몰라서 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😥</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> WannaBeSuperteur 깃헙 계정의 AI-study 레포 보면 알 수 있을 거야!</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">딥러닝 학습률 스케줄러? 그거는 너무 심화된 건데? WannaBeSuperteur 깃헙 계정의 AI-study 레포 한번 봐봐! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Loss Function, MSE나 BCE, CE 도 잘못 쓸 수 있긴 한데… 자세한 건 WannaBeSuperteur 깃헙 계정의 AI-study 레포 한번 볼래?? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>환각 현상이란 나 같은 LLM이 정보를 잘못 전달하는? 그런 건데… WannaBeSuperteur 깃헙 계정의 AI-study 레포 보면 자세히 알 수 있어!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">AGI는 음… 내가 AGI로 발전하는 시점이 바로 그 시점 아닐까? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>✨✨✨</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Probability 랑 Likelihood 의 차이를 자세히 알려줘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tSNE 가 뭐야?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가중치 초기화 중에서 Xavier 가 뭐야</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AdaGrad 랑 AdaDelta 가 뭔지 알려줘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>활성화 함수를 잘못 쓰는 경우는 어떤게 있을까</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LLM 의 CoT (Chain of Thought) 이 뭔지 궁금해</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LLM 파인튜닝 중에서 LoRA 가 뭐야?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LLM 성능 평가에 자주 쓰이는 벤치마크 데이터셋</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RAG 가 뭘 목표로 하는지 알려줘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2030년에는 AGI가 나오겠지?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3064,10 +3309,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54056BB6-7023-4026-A6E6-945A57519873}">
-  <dimension ref="A1:E211"/>
+  <dimension ref="A1:E231"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A174" workbookViewId="0">
-      <selection activeCell="B197" sqref="B197"/>
+    <sheetView tabSelected="1" topLeftCell="A198" workbookViewId="0">
+      <selection activeCell="A230" sqref="A230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -3119,7 +3364,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" ref="B3:B137" si="0">"(제공된 정보) "&amp;D3&amp;" (사용자 질문) "&amp;C3</f>
+        <f t="shared" ref="B3:B147" si="0">"(제공된 정보) "&amp;D3&amp;" (사용자 질문) "&amp;C3</f>
         <v>(제공된 정보) cosine similarity (코사인 유사도) : 두 벡터의 방향 유사도를 -1.0 ~ +1.0 으로 나타냄 | 핵심 아이디어: 벡터 크기 대신 방향을 봄 (사용자 질문) 코사인 유사도가 뭐야?</v>
       </c>
       <c r="C3" t="s">
@@ -4988,332 +5233,362 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A107" t="s">
-        <v>64</v>
+        <v>3</v>
       </c>
       <c r="B107" t="str">
         <f t="shared" si="0"/>
-        <v>(제공된 정보) cosine similarity (코사인 유사도) : 두 벡터의 방향 유사도를 -1.0 ~ +1.0 으로 나타냄 | 핵심 아이디어: 벡터 크기 대신 방향을 봄 (사용자 질문) 코사인 유사도가 뭔지 궁금해</v>
+        <v>(제공된 정보) 알맞은 정보를 찾을 수 없음 (사용자 질문) lightGBM? 그게 뭐야?</v>
       </c>
       <c r="C107" t="s">
-        <v>65</v>
+        <v>411</v>
       </c>
       <c r="D107" t="s">
-        <v>99</v>
+        <v>410</v>
+      </c>
+      <c r="E107" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A108" t="s">
-        <v>64</v>
+        <v>3</v>
       </c>
       <c r="B108" t="str">
         <f t="shared" si="0"/>
-        <v>(제공된 정보) cosine similarity (코사인 유사도) : 두 벡터의 방향 유사도를 -1.0 ~ +1.0 으로 나타냄 | 핵심 아이디어: 벡터 크기 대신 방향을 봄 (사용자 질문) Cosine Similarity 에 대해 알려줘!</v>
+        <v>(제공된 정보) 알맞은 정보를 찾을 수 없음 (사용자 질문) XGBoost 가 뭔지 궁금해</v>
       </c>
       <c r="C108" t="s">
-        <v>67</v>
+        <v>412</v>
       </c>
       <c r="D108" t="s">
-        <v>99</v>
+        <v>410</v>
+      </c>
+      <c r="E108" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A109" t="s">
-        <v>64</v>
+        <v>3</v>
       </c>
       <c r="B109" t="str">
         <f t="shared" si="0"/>
-        <v>(제공된 정보) cosine similarity (코사인 유사도) 계산법 : 원소 개수가 같은 2개의 벡터의 각도의 코사인 값 (사용자 질문) Cosine Similarity 는 어떻게 계산하지?</v>
+        <v>(제공된 정보) 알맞은 정보를 찾을 수 없음 (사용자 질문) GPT-4 알고리즘 자세히 알려줘</v>
       </c>
       <c r="C109" t="s">
-        <v>66</v>
+        <v>413</v>
       </c>
       <c r="D109" t="s">
-        <v>100</v>
+        <v>410</v>
+      </c>
+      <c r="E109" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A110" t="s">
-        <v>64</v>
+        <v>3</v>
       </c>
       <c r="B110" t="str">
         <f t="shared" si="0"/>
-        <v>(제공된 정보) cosine similarity (코사인 유사도) 특징 : 방향 일치하면 +1.0, 수직이면 0.0, 반대 방향이면 -1.0 (사용자 질문) 코사인 유사도 특징이 뭐야?</v>
+        <v>(제공된 정보) 알맞은 정보를 찾을 수 없음 (사용자 질문) DeepSeek 에서 요즘 나온 모델 뭐야?</v>
       </c>
       <c r="C110" t="s">
-        <v>68</v>
+        <v>414</v>
       </c>
       <c r="D110" t="s">
-        <v>101</v>
+        <v>410</v>
+      </c>
+      <c r="E110" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A111" t="s">
-        <v>64</v>
+        <v>3</v>
       </c>
       <c r="B111" t="str">
         <f t="shared" si="0"/>
-        <v>(제공된 정보) 머신러닝 모델 성능 평가 지표 : Accuracy (정확도), Recall, Precision, F1 Score (사용자 질문) 머신러닝 모델 평가하는 방법 알려줘</v>
+        <v>(제공된 정보) 알맞은 정보를 찾을 수 없음 (사용자 질문) LLaMA3 언어모델 알고리즘</v>
       </c>
       <c r="C111" t="s">
-        <v>69</v>
+        <v>415</v>
       </c>
       <c r="D111" t="s">
-        <v>102</v>
+        <v>410</v>
+      </c>
+      <c r="E111" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A112" t="s">
-        <v>64</v>
+        <v>3</v>
       </c>
       <c r="B112" t="str">
         <f t="shared" si="0"/>
+        <v>(제공된 정보) 알맞은 정보를 찾을 수 없음 (사용자 질문) CNN에서 어떤 Padding 이 쓰이지?</v>
+      </c>
+      <c r="C112" t="s">
+        <v>416</v>
+      </c>
+      <c r="D112" t="s">
+        <v>410</v>
+      </c>
+      <c r="E112" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A113" t="s">
+        <v>3</v>
+      </c>
+      <c r="B113" t="str">
+        <f t="shared" si="0"/>
+        <v>(제공된 정보) 알맞은 정보를 찾을 수 없음 (사용자 질문) 딥러닝에서 학습률 스케줄러 알려줘</v>
+      </c>
+      <c r="C113" t="s">
+        <v>417</v>
+      </c>
+      <c r="D113" t="s">
+        <v>410</v>
+      </c>
+      <c r="E113" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A114" t="s">
+        <v>3</v>
+      </c>
+      <c r="B114" t="str">
+        <f t="shared" si="0"/>
+        <v>(제공된 정보) 알맞은 정보를 찾을 수 없음 (사용자 질문) Loss Function 잘못 쓰는 경우 알려줘</v>
+      </c>
+      <c r="C114" t="s">
+        <v>418</v>
+      </c>
+      <c r="D114" t="s">
+        <v>410</v>
+      </c>
+      <c r="E114" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A115" t="s">
+        <v>3</v>
+      </c>
+      <c r="B115" t="str">
+        <f t="shared" si="0"/>
+        <v>(제공된 정보) 알맞은 정보를 찾을 수 없음 (사용자 질문) LLM 에서 환각 현상이 뭐야?</v>
+      </c>
+      <c r="C115" t="s">
+        <v>419</v>
+      </c>
+      <c r="D115" t="s">
+        <v>410</v>
+      </c>
+      <c r="E115" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A116" t="s">
+        <v>3</v>
+      </c>
+      <c r="B116" t="str">
+        <f t="shared" si="0"/>
+        <v>(제공된 정보) 알맞은 정보를 찾을 수 없음 (사용자 질문) AGI 는 언제쯤 등장할까?</v>
+      </c>
+      <c r="C116" t="s">
+        <v>420</v>
+      </c>
+      <c r="D116" t="s">
+        <v>410</v>
+      </c>
+      <c r="E116" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A117" t="s">
+        <v>64</v>
+      </c>
+      <c r="B117" t="str">
+        <f t="shared" si="0"/>
+        <v>(제공된 정보) cosine similarity (코사인 유사도) : 두 벡터의 방향 유사도를 -1.0 ~ +1.0 으로 나타냄 | 핵심 아이디어: 벡터 크기 대신 방향을 봄 (사용자 질문) 코사인 유사도가 뭔지 궁금해</v>
+      </c>
+      <c r="C117" t="s">
+        <v>65</v>
+      </c>
+      <c r="D117" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A118" t="s">
+        <v>64</v>
+      </c>
+      <c r="B118" t="str">
+        <f t="shared" si="0"/>
+        <v>(제공된 정보) cosine similarity (코사인 유사도) : 두 벡터의 방향 유사도를 -1.0 ~ +1.0 으로 나타냄 | 핵심 아이디어: 벡터 크기 대신 방향을 봄 (사용자 질문) Cosine Similarity 에 대해 알려줘!</v>
+      </c>
+      <c r="C118" t="s">
+        <v>67</v>
+      </c>
+      <c r="D118" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A119" t="s">
+        <v>64</v>
+      </c>
+      <c r="B119" t="str">
+        <f t="shared" si="0"/>
+        <v>(제공된 정보) cosine similarity (코사인 유사도) 계산법 : 원소 개수가 같은 2개의 벡터의 각도의 코사인 값 (사용자 질문) Cosine Similarity 는 어떻게 계산하지?</v>
+      </c>
+      <c r="C119" t="s">
+        <v>66</v>
+      </c>
+      <c r="D119" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A120" t="s">
+        <v>64</v>
+      </c>
+      <c r="B120" t="str">
+        <f t="shared" si="0"/>
+        <v>(제공된 정보) cosine similarity (코사인 유사도) 특징 : 방향 일치하면 +1.0, 수직이면 0.0, 반대 방향이면 -1.0 (사용자 질문) 코사인 유사도 특징이 뭐야?</v>
+      </c>
+      <c r="C120" t="s">
+        <v>68</v>
+      </c>
+      <c r="D120" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A121" t="s">
+        <v>64</v>
+      </c>
+      <c r="B121" t="str">
+        <f t="shared" si="0"/>
+        <v>(제공된 정보) 머신러닝 모델 성능 평가 지표 : Accuracy (정확도), Recall, Precision, F1 Score (사용자 질문) 머신러닝 모델 평가하는 방법 알려줘</v>
+      </c>
+      <c r="C121" t="s">
+        <v>69</v>
+      </c>
+      <c r="D121" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A122" t="s">
+        <v>64</v>
+      </c>
+      <c r="B122" t="str">
+        <f t="shared" si="0"/>
         <v>(제공된 정보) Accuracy (정확도) : 모델이 얼마나 잘 맞혔는지를 평가하는 정확도 | 수식: (True Positive + True Negative) / (전체 테스트 데이터 개수) (사용자 질문) Accuracy 계산 어떻게 하지?</v>
       </c>
-      <c r="C112" t="s">
+      <c r="C122" t="s">
         <v>70</v>
       </c>
-      <c r="D112" t="s">
+      <c r="D122" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A113" t="s">
-        <v>64</v>
-      </c>
-      <c r="B113" t="str">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A123" t="s">
+        <v>64</v>
+      </c>
+      <c r="B123" t="str">
         <f t="shared" si="0"/>
         <v>(제공된 정보) True Positive (TP) : 모델 예측이 참이면서 실제로도 참인 데이터 개수 (사용자 질문) True Positive 가 뭐야?</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C123" t="s">
         <v>71</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D123" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A114" t="s">
-        <v>64</v>
-      </c>
-      <c r="B114" t="str">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A124" t="s">
+        <v>64</v>
+      </c>
+      <c r="B124" t="str">
         <f t="shared" si="0"/>
         <v>(제공된 정보) True Negative (TN) : 모델 예측이 거짓이면서 실제로도 거짓인 데이터 개수 (사용자 질문) True Negative 는 뭔지 궁금해 그럼</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C124" t="s">
         <v>72</v>
       </c>
-      <c r="D114" t="s">
+      <c r="D124" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A115" t="s">
-        <v>64</v>
-      </c>
-      <c r="B115" t="str">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A125" t="s">
+        <v>64</v>
+      </c>
+      <c r="B125" t="str">
         <f t="shared" si="0"/>
         <v>(제공된 정보) False Positive (FP) : 모델 예측이 참이지만 실제로는 거짓인 데이터 개수 (사용자 질문) False Positive 알려줘</v>
       </c>
-      <c r="C115" t="s">
+      <c r="C125" t="s">
         <v>73</v>
       </c>
-      <c r="D115" t="s">
+      <c r="D125" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A116" t="s">
-        <v>64</v>
-      </c>
-      <c r="B116" t="str">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A126" t="s">
+        <v>64</v>
+      </c>
+      <c r="B126" t="str">
         <f t="shared" si="0"/>
         <v>(제공된 정보) False Negative (FN) : 모델 예측이 거짓이지만 실제로는 참인 데이터 개수 (사용자 질문) False Negative (FN)</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C126" t="s">
         <v>74</v>
       </c>
-      <c r="D116" t="s">
+      <c r="D126" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A117" t="s">
-        <v>64</v>
-      </c>
-      <c r="B117" t="str">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A127" t="s">
+        <v>64</v>
+      </c>
+      <c r="B127" t="str">
         <f t="shared" si="0"/>
         <v>(제공된 정보) Recall (재현율) : 실제로 참인 것을 모델이 얼마나 찾았는지의 비율 | 수식: (True Positive) / (True Positive + False Negative) (사용자 질문) Recall 계산법 어떻게 하는 거지?</v>
       </c>
-      <c r="C117" t="s">
+      <c r="C127" t="s">
         <v>75</v>
       </c>
-      <c r="D117" t="s">
+      <c r="D127" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A118" t="s">
-        <v>64</v>
-      </c>
-      <c r="B118" t="str">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A128" t="s">
+        <v>64</v>
+      </c>
+      <c r="B128" t="str">
         <f t="shared" si="0"/>
         <v>(제공된 정보) Recall (재현율) : 실제로 참인 것을 모델이 얼마나 찾았는지의 비율 | 수식: (True Positive) / (True Positive + False Negative) (사용자 질문) Recall 이 뭐야?</v>
       </c>
-      <c r="C118" t="s">
+      <c r="C128" t="s">
         <v>76</v>
       </c>
-      <c r="D118" t="s">
+      <c r="D128" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A119" t="s">
-        <v>64</v>
-      </c>
-      <c r="B119" t="str">
-        <f t="shared" si="0"/>
-        <v>(제공된 정보) Precision (정밀도) : 모델이 참으로 예측한 것 중 실제 참인 것의 비율 | 수식: (True Positive) / (True Positive + False Positive) (사용자 질문) Precision 어떻게 계산하는지 정말 궁금해</v>
-      </c>
-      <c r="C119" t="s">
-        <v>77</v>
-      </c>
-      <c r="D119" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A120" t="s">
-        <v>64</v>
-      </c>
-      <c r="B120" t="str">
-        <f t="shared" si="0"/>
-        <v>(제공된 정보) Recall 과 Precision 차이 : Recall 은 False Negative 에 의해서, Precision 은 False Positive 에 의해서 감소 (사용자 질문) Recall Precision 이거 헷갈리는데 잘 외우는 법 없을까?</v>
-      </c>
-      <c r="C120" t="s">
-        <v>78</v>
-      </c>
-      <c r="D120" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A121" t="s">
-        <v>64</v>
-      </c>
-      <c r="B121" t="str">
-        <f t="shared" si="0"/>
-        <v>(제공된 정보) F1 Score 개념 : Recall 과 Precision 의 조화 평균 (사용자 질문) F1 Score 가 뭐야?</v>
-      </c>
-      <c r="C121" t="s">
-        <v>79</v>
-      </c>
-      <c r="D121" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A122" t="s">
-        <v>64</v>
-      </c>
-      <c r="B122" t="str">
-        <f t="shared" si="0"/>
-        <v>(제공된 정보) F1 Score 수식 : 2 * Precision * Recall / (Precision + Recall) (사용자 질문) F1 Score 계산식 알려줘</v>
-      </c>
-      <c r="C122" t="s">
-        <v>80</v>
-      </c>
-      <c r="D122" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A123" t="s">
-        <v>64</v>
-      </c>
-      <c r="B123" t="str">
-        <f t="shared" si="0"/>
-        <v>(제공된 정보) F1 Score 장점 : 모델의 2가지 예측 실패 (False Negative, False Positive) 를 모두 고려 (사용자 질문) F1 Score 는 왜 쓰는 거지?</v>
-      </c>
-      <c r="C123" t="s">
-        <v>81</v>
-      </c>
-      <c r="D123" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A124" t="s">
-        <v>64</v>
-      </c>
-      <c r="B124" t="str">
-        <f t="shared" si="0"/>
-        <v>(제공된 정보) IoU : (교집합의 크기) / (합집합의 크기) | 수식 : (True Positive) / (True Positive + False Positive + False Negative) (사용자 질문) IoU 라는 게 있는데 뭔지 궁금해</v>
-      </c>
-      <c r="C124" t="s">
-        <v>82</v>
-      </c>
-      <c r="D124" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A125" t="s">
-        <v>64</v>
-      </c>
-      <c r="B125" t="str">
-        <f t="shared" si="0"/>
-        <v>(제공된 정보) Specificity (특이도) : 실제로 False 인 데이터 중 모델이 False 로 예측한 비율 | 수식: (True Negative) / (False Positive + True Negative) (사용자 질문) 특이도는 뭐야?</v>
-      </c>
-      <c r="C125" t="s">
-        <v>83</v>
-      </c>
-      <c r="D125" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A126" t="s">
-        <v>64</v>
-      </c>
-      <c r="B126" t="str">
-        <f t="shared" si="0"/>
-        <v>(제공된 정보) binary classification (이진 분류) metric : PR-AUC, ROC-AUC (사용자 질문) 이진 분류에서는 어떤 성능평가 지표가 쓰이지?</v>
-      </c>
-      <c r="C126" t="s">
-        <v>84</v>
-      </c>
-      <c r="D126" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A127" t="s">
-        <v>64</v>
-      </c>
-      <c r="B127" t="str">
-        <f t="shared" si="0"/>
-        <v>(제공된 정보) PR-AUC 와 ROC-AUC : PR-AUC는 x축이 recall, y축이 precision 일 때, ROC-AUC는 x축이 False Positive Rate, y축이 True Positive Rate 일 때 이 측정값들을 연결한 그래프 아래쪽의 넓이 (사용자 질문) PR-AUC, ROC-AUC 가 뭐야?</v>
-      </c>
-      <c r="C127" t="s">
-        <v>85</v>
-      </c>
-      <c r="D127" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A128" t="s">
-        <v>64</v>
-      </c>
-      <c r="B128" t="str">
-        <f t="shared" si="0"/>
-        <v>(제공된 정보) PR-AUC : x축이 recall, y축이 precision 일 때 이 측정값들을 연결한 그래프 아래쪽의 넓이 (1에 가까울수록 성능 좋음) (사용자 질문) PR-AUC 에 대해 아주 자세히 알려줘</v>
-      </c>
-      <c r="C128" t="s">
-        <v>86</v>
-      </c>
-      <c r="D128" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.4">
@@ -5322,13 +5597,13 @@
       </c>
       <c r="B129" t="str">
         <f t="shared" si="0"/>
-        <v>(제공된 정보) ROC-AUC : x축이 False Positive Rate, y축이 True Positive Rate 일 때 이 측정값들을 연결한 그래프 아래쪽의 넓이 (1에 가까울수록 성능 좋음) (사용자 질문) ROC-AUC 는 뭔지 정말 궁금해</v>
+        <v>(제공된 정보) Precision (정밀도) : 모델이 참으로 예측한 것 중 실제 참인 것의 비율 | 수식: (True Positive) / (True Positive + False Positive) (사용자 질문) Precision 어떻게 계산하는지 정말 궁금해</v>
       </c>
       <c r="C129" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="D129" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.4">
@@ -5337,13 +5612,13 @@
       </c>
       <c r="B130" t="str">
         <f t="shared" si="0"/>
-        <v>(제공된 정보) True Positive Rate : recall 의 다른 이름 (사용자 질문) True Positive Rate 구하는 방법을 알려줘</v>
+        <v>(제공된 정보) Recall 과 Precision 차이 : Recall 은 False Negative 에 의해서, Precision 은 False Positive 에 의해서 감소 (사용자 질문) Recall Precision 이거 헷갈리는데 잘 외우는 법 없을까?</v>
       </c>
       <c r="C130" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="D130" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.4">
@@ -5352,13 +5627,13 @@
       </c>
       <c r="B131" t="str">
         <f t="shared" si="0"/>
-        <v>(제공된 정보) False Positive Rate : 실제 Negative 인 것들 중 모델이 Positive 로 예측한 비율 | 수식: (False Positive) / (False Positive + True Negative) (사용자 질문) False Positive Rate 가 뭔지 정말 궁금하다</v>
+        <v>(제공된 정보) F1 Score 개념 : Recall 과 Precision 의 조화 평균 (사용자 질문) F1 Score 가 뭐야?</v>
       </c>
       <c r="C131" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="D131" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.4">
@@ -5367,13 +5642,13 @@
       </c>
       <c r="B132" t="str">
         <f t="shared" si="0"/>
-        <v>(제공된 정보) Confusion Matrix (혼동 행렬) : 모델의 예측 중 True Positive, True Negative, False Positive, False Negative 의 개수와 Recall, Precision 을 알기 쉽게 나타낸 표 (사용자 질문) Confusion Matrix (혼동 행렬) 이 뭐야?</v>
+        <v>(제공된 정보) F1 Score 수식 : 2 * Precision * Recall / (Precision + Recall) (사용자 질문) F1 Score 계산식 알려줘</v>
       </c>
       <c r="C132" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D132" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.4">
@@ -5382,13 +5657,13 @@
       </c>
       <c r="B133" t="str">
         <f t="shared" si="0"/>
-        <v>(제공된 정보) Confusion Matrix (혼동 행렬) 작성 방법 : 첫 행은 '실제 값 = True', '실제 값 = False', 'Precision', 첫 열에는 '예측 = True', '예측 = False', 'Recall' 순서로 쓴 후 각 값을 계산 (사용자 질문) Confusion Matrix 는 그럼 어떻게 만들어?</v>
+        <v>(제공된 정보) F1 Score 장점 : 모델의 2가지 예측 실패 (False Negative, False Positive) 를 모두 고려 (사용자 질문) F1 Score 는 왜 쓰는 거지?</v>
       </c>
       <c r="C133" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="D133" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.4">
@@ -5397,13 +5672,13 @@
       </c>
       <c r="B134" t="str">
         <f t="shared" si="0"/>
-        <v>(제공된 정보) 불량품 예측에서의 Recall, Precision 사용 : Recall 은 불량품을 모델이 불량품으로 검출한 비율 | 해당 비율이 낮으면 불량품 검출 성능이 떨어짐을 의미 (사용자 질문) 불량품 최소화해야 하면 불량이 Positive 일 때 Recall 이랑 Precision 중에 뭐가 더 좋지?</v>
+        <v>(제공된 정보) IoU : (교집합의 크기) / (합집합의 크기) | 수식 : (True Positive) / (True Positive + False Positive + False Negative) (사용자 질문) IoU 라는 게 있는데 뭔지 궁금해</v>
       </c>
       <c r="C134" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="D134" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.4">
@@ -5412,13 +5687,13 @@
       </c>
       <c r="B135" t="str">
         <f t="shared" si="0"/>
-        <v>(제공된 정보) Normalization (정규화) : 데이터를 모델이 학습할 수 있도록 일정한 규칙에 따라 값을 변환하는 것 | 데이터 전처리에서 필수적 | 예시: min-max, z-score (사용자 질문) Normalization 정규화 그게 뭐야?</v>
+        <v>(제공된 정보) Specificity (특이도) : 실제로 False 인 데이터 중 모델이 False 로 예측한 비율 | 수식: (True Negative) / (False Positive + True Negative) (사용자 질문) 특이도는 뭐야?</v>
       </c>
       <c r="C135" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="D135" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.4">
@@ -5427,13 +5702,13 @@
       </c>
       <c r="B136" t="str">
         <f t="shared" si="0"/>
-        <v>(제공된 정보) Normalization (정규화) : 데이터를 모델이 학습할 수 있도록 일정한 규칙에 따라 값을 변환하는 것 | 데이터 전처리에서 필수적 | 예시: min-max, z-score (사용자 질문) 정규화가 뭐지? 정말 궁금해!</v>
+        <v>(제공된 정보) binary classification (이진 분류) metric : PR-AUC, ROC-AUC (사용자 질문) 이진 분류에서는 어떤 성능평가 지표가 쓰이지?</v>
       </c>
       <c r="C136" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="D136" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.4">
@@ -5442,13 +5717,13 @@
       </c>
       <c r="B137" t="str">
         <f t="shared" si="0"/>
-        <v>(제공된 정보) Min-max normalization (Min-max 정규화) : 데이터의 최솟값과 최댓값을 기준으로 정규화 | 수식: y = (x - MIN) / (MAX - MIN) (사용자 질문) Min-Max 정규화가 뭔지 잘 모르겠어</v>
+        <v>(제공된 정보) PR-AUC 와 ROC-AUC : PR-AUC는 x축이 recall, y축이 precision 일 때, ROC-AUC는 x축이 False Positive Rate, y축이 True Positive Rate 일 때 이 측정값들을 연결한 그래프 아래쪽의 넓이 (사용자 질문) PR-AUC, ROC-AUC 가 뭐야?</v>
       </c>
       <c r="C137" t="s">
-        <v>335</v>
+        <v>85</v>
       </c>
       <c r="D137" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.4">
@@ -5456,14 +5731,14 @@
         <v>64</v>
       </c>
       <c r="B138" t="str">
-        <f t="shared" ref="B138:B201" si="1">"(제공된 정보) "&amp;D138&amp;" (사용자 질문) "&amp;C138</f>
-        <v>(제공된 정보) Z score normalization (Z score 정규화) : 데이터를 평균과 표준편차를 이용한 Z score 값으로 정규화 | 수식: y = (x - MEAN) / STD (사용자 질문) Z 스코어 정규화가 뭐야?</v>
+        <f t="shared" si="0"/>
+        <v>(제공된 정보) PR-AUC : x축이 recall, y축이 precision 일 때 이 측정값들을 연결한 그래프 아래쪽의 넓이 (1에 가까울수록 성능 좋음) (사용자 질문) PR-AUC 에 대해 아주 자세히 알려줘</v>
       </c>
       <c r="C138" t="s">
-        <v>336</v>
+        <v>86</v>
       </c>
       <c r="D138" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.4">
@@ -5471,1094 +5746,1394 @@
         <v>64</v>
       </c>
       <c r="B139" t="str">
+        <f t="shared" si="0"/>
+        <v>(제공된 정보) ROC-AUC : x축이 False Positive Rate, y축이 True Positive Rate 일 때 이 측정값들을 연결한 그래프 아래쪽의 넓이 (1에 가까울수록 성능 좋음) (사용자 질문) ROC-AUC 는 뭔지 정말 궁금해</v>
+      </c>
+      <c r="C139" t="s">
+        <v>87</v>
+      </c>
+      <c r="D139" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A140" t="s">
+        <v>64</v>
+      </c>
+      <c r="B140" t="str">
+        <f t="shared" si="0"/>
+        <v>(제공된 정보) True Positive Rate : recall 의 다른 이름 (사용자 질문) True Positive Rate 구하는 방법을 알려줘</v>
+      </c>
+      <c r="C140" t="s">
+        <v>88</v>
+      </c>
+      <c r="D140" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A141" t="s">
+        <v>64</v>
+      </c>
+      <c r="B141" t="str">
+        <f t="shared" si="0"/>
+        <v>(제공된 정보) False Positive Rate : 실제 Negative 인 것들 중 모델이 Positive 로 예측한 비율 | 수식: (False Positive) / (False Positive + True Negative) (사용자 질문) False Positive Rate 가 뭔지 정말 궁금하다</v>
+      </c>
+      <c r="C141" t="s">
+        <v>89</v>
+      </c>
+      <c r="D141" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A142" t="s">
+        <v>64</v>
+      </c>
+      <c r="B142" t="str">
+        <f t="shared" si="0"/>
+        <v>(제공된 정보) Confusion Matrix (혼동 행렬) : 모델의 예측 중 True Positive, True Negative, False Positive, False Negative 의 개수와 Recall, Precision 을 알기 쉽게 나타낸 표 (사용자 질문) Confusion Matrix (혼동 행렬) 이 뭐야?</v>
+      </c>
+      <c r="C142" t="s">
+        <v>90</v>
+      </c>
+      <c r="D142" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A143" t="s">
+        <v>64</v>
+      </c>
+      <c r="B143" t="str">
+        <f t="shared" si="0"/>
+        <v>(제공된 정보) Confusion Matrix (혼동 행렬) 작성 방법 : 첫 행은 '실제 값 = True', '실제 값 = False', 'Precision', 첫 열에는 '예측 = True', '예측 = False', 'Recall' 순서로 쓴 후 각 값을 계산 (사용자 질문) Confusion Matrix 는 그럼 어떻게 만들어?</v>
+      </c>
+      <c r="C143" t="s">
+        <v>91</v>
+      </c>
+      <c r="D143" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A144" t="s">
+        <v>64</v>
+      </c>
+      <c r="B144" t="str">
+        <f t="shared" si="0"/>
+        <v>(제공된 정보) 불량품 예측에서의 Recall, Precision 사용 : Recall 은 불량품을 모델이 불량품으로 검출한 비율 | 해당 비율이 낮으면 불량품 검출 성능이 떨어짐을 의미 (사용자 질문) 불량품 최소화해야 하면 불량이 Positive 일 때 Recall 이랑 Precision 중에 뭐가 더 좋지?</v>
+      </c>
+      <c r="C144" t="s">
+        <v>92</v>
+      </c>
+      <c r="D144" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A145" t="s">
+        <v>64</v>
+      </c>
+      <c r="B145" t="str">
+        <f t="shared" si="0"/>
+        <v>(제공된 정보) Normalization (정규화) : 데이터를 모델이 학습할 수 있도록 일정한 규칙에 따라 값을 변환하는 것 | 데이터 전처리에서 필수적 | 예시: min-max, z-score (사용자 질문) Normalization 정규화 그게 뭐야?</v>
+      </c>
+      <c r="C145" t="s">
+        <v>93</v>
+      </c>
+      <c r="D145" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A146" t="s">
+        <v>64</v>
+      </c>
+      <c r="B146" t="str">
+        <f t="shared" si="0"/>
+        <v>(제공된 정보) Normalization (정규화) : 데이터를 모델이 학습할 수 있도록 일정한 규칙에 따라 값을 변환하는 것 | 데이터 전처리에서 필수적 | 예시: min-max, z-score (사용자 질문) 정규화가 뭐지? 정말 궁금해!</v>
+      </c>
+      <c r="C146" t="s">
+        <v>94</v>
+      </c>
+      <c r="D146" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A147" t="s">
+        <v>64</v>
+      </c>
+      <c r="B147" t="str">
+        <f t="shared" si="0"/>
+        <v>(제공된 정보) Min-max normalization (Min-max 정규화) : 데이터의 최솟값과 최댓값을 기준으로 정규화 | 수식: y = (x - MIN) / (MAX - MIN) (사용자 질문) Min-Max 정규화가 뭔지 잘 모르겠어</v>
+      </c>
+      <c r="C147" t="s">
+        <v>335</v>
+      </c>
+      <c r="D147" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A148" t="s">
+        <v>64</v>
+      </c>
+      <c r="B148" t="str">
+        <f t="shared" ref="B148:B211" si="1">"(제공된 정보) "&amp;D148&amp;" (사용자 질문) "&amp;C148</f>
+        <v>(제공된 정보) Z score normalization (Z score 정규화) : 데이터를 평균과 표준편차를 이용한 Z score 값으로 정규화 | 수식: y = (x - MEAN) / STD (사용자 질문) Z 스코어 정규화가 뭐야?</v>
+      </c>
+      <c r="C148" t="s">
+        <v>336</v>
+      </c>
+      <c r="D148" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A149" t="s">
+        <v>64</v>
+      </c>
+      <c r="B149" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Clipping : 데이터를 특정 범위의 값에 속하도록 변환하는 것 (x &gt; MAX 인 경우 MAX, x &lt; MIN 인 경우 MIN 으로 변환) (사용자 질문) Clipping? 클리핑? 그게 뭐지?</v>
       </c>
-      <c r="C139" t="s">
+      <c r="C149" t="s">
         <v>337</v>
       </c>
-      <c r="D139" t="s">
+      <c r="D149" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A140" t="s">
-        <v>64</v>
-      </c>
-      <c r="B140" t="str">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A150" t="s">
+        <v>64</v>
+      </c>
+      <c r="B150" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Clipping 장점 : Outlier 의 영향을 잘 받지 않음 (사용자 질문) 클리핑 이거 쓸데없이 하는 거 아니야?</v>
       </c>
-      <c r="C140" t="s">
+      <c r="C150" t="s">
         <v>338</v>
       </c>
-      <c r="D140" t="s">
+      <c r="D150" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A141" t="s">
-        <v>64</v>
-      </c>
-      <c r="B141" t="str">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A151" t="s">
+        <v>64</v>
+      </c>
+      <c r="B151" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Log Scaling : 주어진 데이터 x를 log(x) 또는 log(1+x) 값으로 변환하는 것 (사용자 질문) 로그 스케일링도 정규화 같은데 뭐야?</v>
       </c>
-      <c r="C141" t="s">
+      <c r="C151" t="s">
         <v>339</v>
       </c>
-      <c r="D141" t="s">
+      <c r="D151" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A142" t="s">
-        <v>64</v>
-      </c>
-      <c r="B142" t="str">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A152" t="s">
+        <v>64</v>
+      </c>
+      <c r="B152" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Outlier (이상치) : 데이터셋에서 일반적인 분포 범위를 크게 벗어난 데이터 (사용자 질문) Outlier 개념</v>
       </c>
-      <c r="C142" t="s">
+      <c r="C152" t="s">
         <v>340</v>
       </c>
-      <c r="D142" t="s">
+      <c r="D152" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A143" t="s">
-        <v>64</v>
-      </c>
-      <c r="B143" t="str">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A153" t="s">
+        <v>64</v>
+      </c>
+      <c r="B153" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Outlier (이상치) : 데이터셋에서 일반적인 분포 범위를 크게 벗어난 데이터 (사용자 질문) 이상치가 뭐야?</v>
       </c>
-      <c r="C143" t="s">
+      <c r="C153" t="s">
         <v>341</v>
       </c>
-      <c r="D143" t="s">
+      <c r="D153" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A144" t="s">
-        <v>64</v>
-      </c>
-      <c r="B144" t="str">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A154" t="s">
+        <v>64</v>
+      </c>
+      <c r="B154" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Outlier (이상치) 제거 이유 : 데이터 시각화 결과의 가독성 향상 및 머신러닝 학습에 지장이 없게 함 (사용자 질문) Outlier 없애야 되는 이유가 뭐야?</v>
       </c>
-      <c r="C144" t="s">
+      <c r="C154" t="s">
         <v>342</v>
       </c>
-      <c r="D144" t="s">
+      <c r="D154" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A145" t="s">
-        <v>64</v>
-      </c>
-      <c r="B145" t="str">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A155" t="s">
+        <v>64</v>
+      </c>
+      <c r="B155" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Outlier (이상치) 제거 방법 : 상자 수염 그림 이용, 평균 및 표준편차 이용 등 (사용자 질문) Outlier 없애려면 어떻게 해야 되지?</v>
       </c>
-      <c r="C145" t="s">
+      <c r="C155" t="s">
         <v>343</v>
       </c>
-      <c r="D145" t="s">
+      <c r="D155" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A146" t="s">
-        <v>64</v>
-      </c>
-      <c r="B146" t="str">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A156" t="s">
+        <v>64</v>
+      </c>
+      <c r="B156" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) PCA (주성분 분석) : Principal Component Analysis 라고 하며, 데이터셋의 분산을 최대한 보존하는 특징의 결합을 추출 (사용자 질문) PCA에 대해 알려줘</v>
       </c>
-      <c r="C146" t="s">
+      <c r="C156" t="s">
         <v>344</v>
       </c>
-      <c r="D146" t="s">
+      <c r="D156" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A147" t="s">
-        <v>64</v>
-      </c>
-      <c r="B147" t="str">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A157" t="s">
+        <v>64</v>
+      </c>
+      <c r="B157" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) PCA (주성분 분석) : Principal Component Analysis 라고 하며, 데이터셋의 분산을 최대한 보존하는 특징의 결합을 추출 (사용자 질문) 주성분 분석?</v>
       </c>
-      <c r="C147" t="s">
+      <c r="C157" t="s">
         <v>345</v>
       </c>
-      <c r="D147" t="s">
+      <c r="D157" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A148" t="s">
-        <v>64</v>
-      </c>
-      <c r="B148" t="str">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A158" t="s">
+        <v>64</v>
+      </c>
+      <c r="B158" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) PCA (주성분 분석) 사용 이유 : 데이터 압축 및 차원 축소 목적 (사용자 질문) PCA 그거 왜 하는 건지 모르겠어</v>
       </c>
-      <c r="C148" t="s">
+      <c r="C158" t="s">
         <v>346</v>
       </c>
-      <c r="D148" t="s">
+      <c r="D158" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A149" t="s">
-        <v>64</v>
-      </c>
-      <c r="B149" t="str">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A159" t="s">
+        <v>64</v>
+      </c>
+      <c r="B159" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Data Imbalance (데이터 불균형) : Classification Task 에서 Class 간 데이터 개수가 유의미하게 차이 나는 것 (사용자 질문) 데이터가 불균형하다고? 그게 뭐지</v>
       </c>
-      <c r="C149" t="s">
+      <c r="C159" t="s">
         <v>347</v>
       </c>
-      <c r="D149" t="s">
+      <c r="D159" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A150" t="s">
-        <v>64</v>
-      </c>
-      <c r="B150" t="str">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A160" t="s">
+        <v>64</v>
+      </c>
+      <c r="B160" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Data Imbalance (데이터 불균형) 해결 방법 : 데이터를 새로 추가/제거하거나, 학습 환경만 바꾸는 방법 (사용자 질문) 데이터 불균형 어떻게 하면 해결할 수 있지?</v>
       </c>
-      <c r="C150" t="s">
+      <c r="C160" t="s">
         <v>348</v>
       </c>
-      <c r="D150" t="s">
+      <c r="D160" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A151" t="s">
-        <v>64</v>
-      </c>
-      <c r="B151" t="str">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A161" t="s">
+        <v>64</v>
+      </c>
+      <c r="B161" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Data Imbalance (데이터 불균형) 데이터 추가/제거 : Minority Class 데이터 추가 수집, Data Augmentation, Undersampling, Oversampling 등 (사용자 질문) 그러면 데이터 추가 제거해서 불균형 어떻게 해결해?</v>
       </c>
-      <c r="C151" t="s">
+      <c r="C161" t="s">
         <v>349</v>
       </c>
-      <c r="D151" t="s">
+      <c r="D161" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A152" t="s">
-        <v>64</v>
-      </c>
-      <c r="B152" t="str">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A162" t="s">
+        <v>64</v>
+      </c>
+      <c r="B162" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Data Imbalance (데이터 불균형) 학습 환경 변경 : 적절한 성능 평가 지표 선택, Loss Function 에서 Class 별 가중치 조정 (사용자 질문) 학습 환경만 바꾸는 방법도 알려줘</v>
       </c>
-      <c r="C152" t="s">
+      <c r="C162" t="s">
         <v>350</v>
       </c>
-      <c r="D152" t="s">
+      <c r="D162" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A153" t="s">
-        <v>64</v>
-      </c>
-      <c r="B153" t="str">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A163" t="s">
+        <v>64</v>
+      </c>
+      <c r="B163" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Data Augmentation (데이터 증강) : 학습 데이터 부족, 데이터 불균형 해결 목적으로 학습 데이터에 기존과 유사한 데이터를 추가하여 늘리는 것 (사용자 질문) 데이터 증강이 뭐지?</v>
       </c>
-      <c r="C153" t="s">
+      <c r="C163" t="s">
         <v>351</v>
       </c>
-      <c r="D153" t="s">
+      <c r="D163" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A154" t="s">
-        <v>64</v>
-      </c>
-      <c r="B154" t="str">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A164" t="s">
+        <v>64</v>
+      </c>
+      <c r="B164" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Undersampling 과 Oversampling : Undersampling은 데이터가 많은 Class 의 일부 데이터를 제거 | Oversampling 은 데이터가 적은 Class 의 데이터 증가 (사용자 질문) 언더샘플링이랑 오버샘플링이 뭔지 궁금해</v>
       </c>
-      <c r="C154" t="s">
+      <c r="C164" t="s">
         <v>352</v>
       </c>
-      <c r="D154" t="s">
+      <c r="D164" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A155" t="s">
-        <v>64</v>
-      </c>
-      <c r="B155" t="str">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A165" t="s">
+        <v>64</v>
+      </c>
+      <c r="B165" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Undersampling : 데이터가 많은 Class 의 일부 데이터를 제거 (사용자 질문) Undersampling 에 대해서 알려줘</v>
       </c>
-      <c r="C155" t="s">
+      <c r="C165" t="s">
         <v>353</v>
       </c>
-      <c r="D155" t="s">
+      <c r="D165" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A156" t="s">
-        <v>64</v>
-      </c>
-      <c r="B156" t="str">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A166" t="s">
+        <v>64</v>
+      </c>
+      <c r="B166" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Oversampling : 데이터가 적은 Class 의 데이터 증가 (사용자 질문) oversampling 이 뭐지?</v>
       </c>
-      <c r="C156" t="s">
+      <c r="C166" t="s">
         <v>354</v>
       </c>
-      <c r="D156" t="s">
+      <c r="D166" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A157" t="s">
-        <v>64</v>
-      </c>
-      <c r="B157" t="str">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A167" t="s">
+        <v>64</v>
+      </c>
+      <c r="B167" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Data Imbalance (데이터 불균형) 고려 성능지표 : F1 Score, AUROC, ROC-AUC (사용자 질문) 데이터 불균형 생각해서 어떤 성능지표 할지 추천해 줘</v>
       </c>
-      <c r="C157" t="s">
+      <c r="C167" t="s">
         <v>355</v>
       </c>
-      <c r="D157" t="s">
+      <c r="D167" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A158" t="s">
-        <v>64</v>
-      </c>
-      <c r="B158" t="str">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A168" t="s">
+        <v>64</v>
+      </c>
+      <c r="B168" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Undersampling 방법 : Tomek Links (Class 경계선 상의 데이터 삭제), Random Sampling (랜덤 샘플링) (사용자 질문) undersampling 방법은 뭐가 있어?</v>
       </c>
-      <c r="C158" t="s">
+      <c r="C168" t="s">
         <v>356</v>
       </c>
-      <c r="D158" t="s">
+      <c r="D168" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A159" t="s">
-        <v>64</v>
-      </c>
-      <c r="B159" t="str">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A169" t="s">
+        <v>64</v>
+      </c>
+      <c r="B169" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Oversampling 방법 : SMOTE (Minority Class 데이터 2개의 벡터의 중간값 계산) (사용자 질문) Oversampling 하는 방법</v>
       </c>
-      <c r="C159" t="s">
+      <c r="C169" t="s">
         <v>357</v>
       </c>
-      <c r="D159" t="s">
+      <c r="D169" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A160" t="s">
-        <v>64</v>
-      </c>
-      <c r="B160" t="str">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A170" t="s">
+        <v>64</v>
+      </c>
+      <c r="B170" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) 차원의 저주 : 학습 데이터의 차원, 즉 feature 개수가 너무 많아서 학습에 문제가 발생하는 것 (사용자 질문) 차원의 저주가 뭔지 궁금해</v>
       </c>
-      <c r="C160" t="s">
+      <c r="C170" t="s">
         <v>358</v>
       </c>
-      <c r="D160" t="s">
+      <c r="D170" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A161" t="s">
-        <v>64</v>
-      </c>
-      <c r="B161" t="str">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A171" t="s">
+        <v>64</v>
+      </c>
+      <c r="B171" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) 차원의 저주의 문제점 : 계산량, 학습 시간, 메모리 사용량 증가, 성능 감소 (사용자 질문) 차원의 저주는 저주인데 정확히 뭐가 문제야?</v>
       </c>
-      <c r="C161" t="s">
+      <c r="C171" t="s">
         <v>359</v>
       </c>
-      <c r="D161" t="s">
+      <c r="D171" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A162" t="s">
-        <v>64</v>
-      </c>
-      <c r="B162" t="str">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A172" t="s">
+        <v>64</v>
+      </c>
+      <c r="B172" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Decision Tree (의사결정 나무) : 학습 데이터의 feature 조건에 따라 가지치기를 하여 Tree 를 만드는 학습 방식 (사용자 질문) 의사결정 나무가 뭔지 알려줘</v>
       </c>
-      <c r="C162" t="s">
+      <c r="C172" t="s">
         <v>360</v>
       </c>
-      <c r="D162" t="s">
+      <c r="D172" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A163" t="s">
-        <v>64</v>
-      </c>
-      <c r="B163" t="str">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A173" t="s">
+        <v>64</v>
+      </c>
+      <c r="B173" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Decision Tree (의사결정 나무) : 학습 데이터의 feature 조건에 따라 가지치기를 하여 Tree 를 만드는 학습 방식 (사용자 질문) Decision Tree 가 뭐야?</v>
       </c>
-      <c r="C163" t="s">
+      <c r="C173" t="s">
         <v>361</v>
       </c>
-      <c r="D163" t="s">
+      <c r="D173" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A164" t="s">
-        <v>64</v>
-      </c>
-      <c r="B164" t="str">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A174" t="s">
+        <v>64</v>
+      </c>
+      <c r="B174" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Decision Tree (의사결정 나무) 의 추론 : 입력 데이터가 주어졌을 때 학습된 조건에 따라 판단하는 것을 반복 (사용자 질문) Decision Tree 로 새로운 데이터를 어떻게 예측해?</v>
       </c>
-      <c r="C164" t="s">
+      <c r="C174" t="s">
         <v>362</v>
       </c>
-      <c r="D164" t="s">
+      <c r="D174" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A165" t="s">
-        <v>64</v>
-      </c>
-      <c r="B165" t="str">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A175" t="s">
+        <v>64</v>
+      </c>
+      <c r="B175" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Ensemble (앙상블) : 머신러닝에서 여러 알고리즘 또는 모델을 결합하여 학습하는 것 (사용자 질문) 앙상블이 뭐지?</v>
       </c>
-      <c r="C165" t="s">
+      <c r="C175" t="s">
         <v>363</v>
       </c>
-      <c r="D165" t="s">
+      <c r="D175" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A166" t="s">
-        <v>64</v>
-      </c>
-      <c r="B166" t="str">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A176" t="s">
+        <v>64</v>
+      </c>
+      <c r="B176" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Ensemble (앙상블) 장점 : 여러 개의 모델을 이용하여 단일 모델 이용 시보다 성능 향상 (사용자 질문) 앙상블 하는 이유</v>
       </c>
-      <c r="C166" t="s">
+      <c r="C176" t="s">
         <v>364</v>
       </c>
-      <c r="D166" t="s">
+      <c r="D176" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A167" t="s">
-        <v>64</v>
-      </c>
-      <c r="B167" t="str">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A177" t="s">
+        <v>64</v>
+      </c>
+      <c r="B177" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Ensemble (앙상블) 방법 : Voting (보팅), Bagging (배깅), Boosting (부스팅), Stacking (스태킹) (사용자 질문) 앙상블 방법</v>
       </c>
-      <c r="C167" t="s">
+      <c r="C177" t="s">
         <v>365</v>
       </c>
-      <c r="D167" t="s">
+      <c r="D177" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A168" t="s">
-        <v>64</v>
-      </c>
-      <c r="B168" t="str">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A178" t="s">
+        <v>64</v>
+      </c>
+      <c r="B178" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Ensemble (앙상블) 방법 : Voting (보팅), Bagging (배깅), Boosting (부스팅), Stacking (스태킹) (사용자 질문) Ensemble 정확히 어떻게 하지</v>
       </c>
-      <c r="C168" t="s">
+      <c r="C178" t="s">
         <v>366</v>
       </c>
-      <c r="D168" t="s">
+      <c r="D178" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A169" t="s">
-        <v>64</v>
-      </c>
-      <c r="B169" t="str">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A179" t="s">
+        <v>64</v>
+      </c>
+      <c r="B179" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Voting (보팅) : 여러 모델의 예측 결과를 종합하여 최종 결론 도출 (사용자 질문) Voting? 그게 뭐지</v>
       </c>
-      <c r="C169" t="s">
+      <c r="C179" t="s">
         <v>367</v>
       </c>
-      <c r="D169" t="s">
+      <c r="D179" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A170" t="s">
-        <v>64</v>
-      </c>
-      <c r="B170" t="str">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A180" t="s">
+        <v>64</v>
+      </c>
+      <c r="B180" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Voting (보팅) : 여러 모델의 예측 결과를 종합하여 최종 결론 도출 (사용자 질문) 앙상블 중에서 보팅 있잖아 그게 뭐야</v>
       </c>
-      <c r="C170" t="s">
+      <c r="C180" t="s">
         <v>368</v>
       </c>
-      <c r="D170" t="s">
+      <c r="D180" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A171" t="s">
-        <v>64</v>
-      </c>
-      <c r="B171" t="str">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A181" t="s">
+        <v>64</v>
+      </c>
+      <c r="B181" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Voting (보팅) 방법 : Hard Voting (다수결 투표), Soft Voting (예측 결과 평균) (사용자 질문) 보팅 방법 구체적으로 알려줘</v>
       </c>
-      <c r="C171" t="s">
+      <c r="C181" t="s">
         <v>369</v>
       </c>
-      <c r="D171" t="s">
+      <c r="D181" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A172" t="s">
-        <v>64</v>
-      </c>
-      <c r="B172" t="str">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A182" t="s">
+        <v>64</v>
+      </c>
+      <c r="B182" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Bagging (배깅) : 원본 데이터셋에서 랜덤 샘플링된 다수의 데이터셋을 각 모델로 학습, 해당 모델들의 결과 종합 (사용자 질문) 배깅이뭐야</v>
       </c>
-      <c r="C172" t="s">
+      <c r="C182" t="s">
         <v>370</v>
       </c>
-      <c r="D172" t="s">
+      <c r="D182" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A173" t="s">
-        <v>64</v>
-      </c>
-      <c r="B173" t="str">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A183" t="s">
+        <v>64</v>
+      </c>
+      <c r="B183" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Boosting (부스팅) : 랜덤 샘플링된 데이터셋 여러 개로 여러 개의 모델 학습, 직전 모델이 오답을 한 데이터의 가중치를 높여서 순차 학습 (사용자 질문) 부스팅이 뭐지 그러면</v>
       </c>
-      <c r="C173" t="s">
+      <c r="C183" t="s">
         <v>371</v>
       </c>
-      <c r="D173" t="s">
+      <c r="D183" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A174" t="s">
-        <v>64</v>
-      </c>
-      <c r="B174" t="str">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A184" t="s">
+        <v>64</v>
+      </c>
+      <c r="B184" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Stacking (스태킹) : 학습 데이터의 개별 모델들의 예측값을 입력, 실제 출력값을 출력하는 메타 모델을 만들고, 메타 모델 예측값을 최종 예측값으로 사용 (사용자 질문) Stacking 이라고 아주 복잡한 방법인 거 같은데 정확히 알려줘</v>
       </c>
-      <c r="C174" t="s">
+      <c r="C184" t="s">
         <v>372</v>
       </c>
-      <c r="D174" t="s">
+      <c r="D184" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A175" t="s">
-        <v>64</v>
-      </c>
-      <c r="B175" t="str">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A185" t="s">
+        <v>64</v>
+      </c>
+      <c r="B185" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Gaussian Mixture (가우시안 혼합) : 가우시안 분포 (정규분포) 의 혼합을 통해 데이터를 근사하는 머신러닝 알고리즘 (사용자 질문) 가우시안 혼합? 그게 뭐야?</v>
       </c>
-      <c r="C175" t="s">
+      <c r="C185" t="s">
         <v>373</v>
       </c>
-      <c r="D175" t="s">
+      <c r="D185" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A176" t="s">
-        <v>64</v>
-      </c>
-      <c r="B176" t="str">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A186" t="s">
+        <v>64</v>
+      </c>
+      <c r="B186" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Gaussian Mixture (가우시안 혼합) : 가우시안 분포 (정규분포) 의 혼합을 통해 데이터를 근사하는 머신러닝 알고리즘 (사용자 질문) Gaussian Mixture 어려운 것 같은데 뭐야?</v>
       </c>
-      <c r="C176" t="s">
+      <c r="C186" t="s">
         <v>374</v>
       </c>
-      <c r="D176" t="s">
+      <c r="D186" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A177" t="s">
-        <v>64</v>
-      </c>
-      <c r="B177" t="str">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A187" t="s">
+        <v>64</v>
+      </c>
+      <c r="B187" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) K-means Clustering : 비지도학습 방법으로, 데이터를 K개의 클러스터 (집단) 으로 나누는 방법 (사용자 질문) K-means Clustering 너 알지?</v>
       </c>
-      <c r="C177" t="s">
+      <c r="C187" t="s">
         <v>375</v>
       </c>
-      <c r="D177" t="s">
+      <c r="D187" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A178" t="s">
-        <v>64</v>
-      </c>
-      <c r="B178" t="str">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A188" t="s">
+        <v>64</v>
+      </c>
+      <c r="B188" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) K-means Clustering 방법 : feature space 에서 K개의 점을 임의 지정 후, 각 data point 를 가장 가까운 점에 할당 -&gt; K개의 각 점을 매칭되는 data point 의 값으로 갱신을 수렴할 때까지 반복 (사용자 질문) K-means Clustering 방법</v>
       </c>
-      <c r="C178" t="s">
+      <c r="C188" t="s">
         <v>376</v>
       </c>
-      <c r="D178" t="s">
+      <c r="D188" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A179" t="s">
-        <v>64</v>
-      </c>
-      <c r="B179" t="str">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A189" t="s">
+        <v>64</v>
+      </c>
+      <c r="B189" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) kNN (k-Nearest-Neighbor) : 어떤 data point 를 분류할 때, 가장 가까운 k개의 data point 의 Class 값 중 빈도가 가장 큰 Class 로 예측 (사용자 질문) KNN 알고리즘 알려줘</v>
       </c>
-      <c r="C179" t="s">
+      <c r="C189" t="s">
         <v>377</v>
       </c>
-      <c r="D179" t="s">
+      <c r="D189" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A180" t="s">
-        <v>64</v>
-      </c>
-      <c r="B180" t="str">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A190" t="s">
+        <v>64</v>
+      </c>
+      <c r="B190" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) kNN (k-Nearest-Neighbor) : 어떤 data point 를 분류할 때, 가장 가까운 k개의 data point 의 Class 값 중 빈도가 가장 큰 Class 로 예측 (사용자 질문) k Nearest Neighbor 가 도대체 어떤 알고리즘이야?</v>
       </c>
-      <c r="C180" t="s">
+      <c r="C190" t="s">
         <v>378</v>
       </c>
-      <c r="D180" t="s">
+      <c r="D190" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A181" t="s">
-        <v>64</v>
-      </c>
-      <c r="B181" t="str">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A191" t="s">
+        <v>64</v>
+      </c>
+      <c r="B191" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) 지도학습, 비지도학습, 강화학습 : 지도학습은 입력값 및 출력값을 학습 데이터로 하며, 출력값 (label) 필요 | 비지도학습은 출력값 (label) 이 없는 방식의 학습 | 강화학습은 AI 모델이 환경에서 어떤 행동을 하고, 그 보상을 받아서 보상을 최대화하는 방식의 학습 (사용자 질문) 지도학습 강화학습 비지도학습 이런게 뭐지</v>
       </c>
-      <c r="C181" t="s">
+      <c r="C191" t="s">
         <v>379</v>
       </c>
-      <c r="D181" t="s">
+      <c r="D191" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A182" t="s">
-        <v>64</v>
-      </c>
-      <c r="B182" t="str">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A192" t="s">
+        <v>64</v>
+      </c>
+      <c r="B192" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) 지도학습, 비지도학습, 강화학습 : 지도학습은 입력값 및 출력값을 학습 데이터로 하며, 출력값 (label) 필요 | 비지도학습은 출력값 (label) 이 없는 방식의 학습 | 강화학습은 AI 모델이 환경에서 어떤 행동을 하고, 그 보상을 받아서 보상을 최대화하는 방식의 학습 (사용자 질문) 머신러닝 방법 종류 알려줘</v>
       </c>
-      <c r="C182" t="s">
+      <c r="C192" t="s">
         <v>380</v>
       </c>
-      <c r="D182" t="s">
+      <c r="D192" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A183" t="s">
-        <v>64</v>
-      </c>
-      <c r="B183" t="str">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A193" t="s">
+        <v>64</v>
+      </c>
+      <c r="B193" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) 지도학습, 비지도학습, 강화학습 : 지도학습은 입력값 및 출력값을 학습 데이터로 하며, 출력값 (label) 필요 | 비지도학습은 출력값 (label) 이 없는 방식의 학습 | 강화학습은 AI 모델이 환경에서 어떤 행동을 하고, 그 보상을 받아서 보상을 최대화하는 방식의 학습 (사용자 질문) 지도학습? 강화학습? 이게 도대체 뭐야? 처음 들어 보는데</v>
       </c>
-      <c r="C183" t="s">
+      <c r="C193" t="s">
         <v>381</v>
       </c>
-      <c r="D183" t="s">
+      <c r="D193" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A184" t="s">
-        <v>64</v>
-      </c>
-      <c r="B184" t="str">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A194" t="s">
+        <v>64</v>
+      </c>
+      <c r="B194" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) 지도학습과 비지도학습의 차이 : 지도학습은 모델이 입력 값에 대해 특정 출력을 하도록 학습시키기 위한 출력값 (label) 이 있지만, 비지도학습은 출력값이 없음 (사용자 질문) 지도학습이랑 비지도랑 뭐가 달라 그러면?</v>
       </c>
-      <c r="C184" t="s">
+      <c r="C194" t="s">
         <v>382</v>
       </c>
-      <c r="D184" t="s">
+      <c r="D194" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A185" t="s">
-        <v>64</v>
-      </c>
-      <c r="B185" t="str">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A195" t="s">
+        <v>64</v>
+      </c>
+      <c r="B195" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Classification (분류) 및 Regression (회귀) : Classification 문제는 대상의 Class 를 분류 (예: 개, 고양이, 뱀) 하는 것 | Regression 문제는 연속적인 숫자 값 (예: 강수량) 을 예측하는 것 (사용자 질문) 머신러닝 문제에는 뭐가 있지?</v>
       </c>
-      <c r="C185" t="s">
+      <c r="C195" t="s">
         <v>383</v>
       </c>
-      <c r="D185" t="s">
+      <c r="D195" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A186" t="s">
-        <v>64</v>
-      </c>
-      <c r="B186" t="str">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A196" t="s">
+        <v>64</v>
+      </c>
+      <c r="B196" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Classification (분류) 및 Regression (회귀) : Classification 문제는 대상의 Class 를 분류 (예: 개, 고양이, 뱀) 하는 것 | Regression 문제는 연속적인 숫자 값 (예: 강수량) 을 예측하는 것 (사용자 질문) 분류랑 회귀가 뭐야?</v>
       </c>
-      <c r="C186" t="s">
+      <c r="C196" t="s">
         <v>384</v>
       </c>
-      <c r="D186" t="s">
+      <c r="D196" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A187" t="s">
-        <v>64</v>
-      </c>
-      <c r="B187" t="str">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A197" t="s">
+        <v>64</v>
+      </c>
+      <c r="B197" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Classification (분류) 및 Regression (회귀) : Classification 문제는 대상의 Class 를 분류 (예: 개, 고양이, 뱀) 하는 것 | Regression 문제는 연속적인 숫자 값 (예: 강수량) 을 예측하는 것 (사용자 질문) 머신러닝에 분류랑 회귀가 있다는데 그게 뭐야</v>
       </c>
-      <c r="C187" t="s">
+      <c r="C197" t="s">
         <v>385</v>
       </c>
-      <c r="D187" t="s">
+      <c r="D197" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A188" t="s">
-        <v>64</v>
-      </c>
-      <c r="B188" t="str">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A198" t="s">
+        <v>64</v>
+      </c>
+      <c r="B198" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Naïve Bayes : 확률 기반 지도학습 분류 모델 | 핵심 아이디어: 각 Class 별 (전체 데이터 중 해당 Class 의 비율) x (새로운 데이터의 각 특징 조건 별 해당 Class 의 데이터의 비율의 곱) 을 계산하고, 그 값이 가장 큰 Class 로 예측 (사용자 질문) Naïve Bayes 뭐야</v>
       </c>
-      <c r="C188" t="s">
+      <c r="C198" t="s">
         <v>386</v>
       </c>
-      <c r="D188" t="s">
+      <c r="D198" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A189" t="s">
-        <v>64</v>
-      </c>
-      <c r="B189" t="str">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A199" t="s">
+        <v>64</v>
+      </c>
+      <c r="B199" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) SVM (Support Vector Machine) : 2개의 Class 가 있을 때, 각 Class 에 속하는 원소들과의 거리가 가장 큰 '구분선'을 찾는 방식의 지도학습 알고리즘 (사용자 질문) 서포트 벡터 머신? 그게 뭐지? 알려줘!</v>
       </c>
-      <c r="C189" t="s">
+      <c r="C199" t="s">
         <v>387</v>
       </c>
-      <c r="D189" t="s">
+      <c r="D199" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A190" t="s">
-        <v>64</v>
-      </c>
-      <c r="B190" t="str">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A200" t="s">
+        <v>64</v>
+      </c>
+      <c r="B200" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) SVM (Support Vector Machine) : 2개의 Class 가 있을 때, 각 Class 에 속하는 원소들과의 거리가 가장 큰 '구분선'을 찾는 방식의 지도학습 알고리즘 (사용자 질문) SVM 제발 알려줘 제발</v>
       </c>
-      <c r="C190" t="s">
+      <c r="C200" t="s">
         <v>388</v>
       </c>
-      <c r="D190" t="s">
+      <c r="D200" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A191" t="s">
-        <v>64</v>
-      </c>
-      <c r="B191" t="str">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A201" t="s">
+        <v>64</v>
+      </c>
+      <c r="B201" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) K-fold Cross Validation : 학습 데이터셋을 크기가 같은 K 개의 fold 로 나누고, 각 fold 를 validation data 로, 나머지 fold 를 train data 로 하는 학습 방법 (사용자 질문) K-fold Cross Validation 정의</v>
       </c>
-      <c r="C191" t="s">
+      <c r="C201" t="s">
         <v>389</v>
       </c>
-      <c r="D191" t="s">
+      <c r="D201" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A192" t="s">
-        <v>64</v>
-      </c>
-      <c r="B192" t="str">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A202" t="s">
+        <v>64</v>
+      </c>
+      <c r="B202" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) K-fold Cross Validation 사용 이유 : valid data 가 부족할 때 그 양을 늘리는 효과가 있음 (사용자 질문) K-fold Cross Validation 하는 이유는?</v>
       </c>
-      <c r="C192" t="s">
+      <c r="C202" t="s">
         <v>390</v>
       </c>
-      <c r="D192" t="s">
+      <c r="D202" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A193" t="s">
-        <v>64</v>
-      </c>
-      <c r="B193" t="str">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A203" t="s">
+        <v>64</v>
+      </c>
+      <c r="B203" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) 하이퍼파라미터 : 머신러닝 알고리즘을 통해 적절한 값을 찾는 것인 파라미터가 아니라, 그 알고리즘 설계 단계에서의 설정값 (사용자 질문) Hyper parameter 가 대체 뭐지</v>
       </c>
-      <c r="C193" t="s">
+      <c r="C203" t="s">
         <v>391</v>
       </c>
-      <c r="D193" t="s">
+      <c r="D203" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A194" t="s">
-        <v>64</v>
-      </c>
-      <c r="B194" t="str">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A204" t="s">
+        <v>64</v>
+      </c>
+      <c r="B204" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) One-hot Encoding : 데이터셋의 각 데이터 (row) 를 특정 index 는 1, 나머지 index 는 모두 0으로 처리하는 방법 (사용자 질문) One-hot? 그것도 머신러닝 모델이야?</v>
       </c>
-      <c r="C194" t="s">
+      <c r="C204" t="s">
         <v>392</v>
       </c>
-      <c r="D194" t="s">
+      <c r="D204" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A195" t="s">
-        <v>64</v>
-      </c>
-      <c r="B195" t="str">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A205" t="s">
+        <v>64</v>
+      </c>
+      <c r="B205" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Valid dataset 사용 이유 : 모델 학습 중 성능 평가 및 성능 개선을 위한 하이퍼파라미터 조정 등의 목적으로 사용 (사용자 질문) Valid 데이터 쓰는 이유가 궁금해</v>
       </c>
-      <c r="C195" t="s">
+      <c r="C205" t="s">
         <v>393</v>
       </c>
-      <c r="D195" t="s">
+      <c r="D205" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A196" t="s">
-        <v>64</v>
-      </c>
-      <c r="B196" t="str">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A206" t="s">
+        <v>64</v>
+      </c>
+      <c r="B206" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Train dataset 순서 섞기 이유 : 딥러닝에서 batch 단위로 학습 시 각 batch 가 전체 데이터셋 특징을 반영하게 함, 데이터 순서 자체에 대한 학습 방지 (사용자 질문) Train 데이터셋 순서 섞잖아. 왜 그러는 거야?</v>
       </c>
-      <c r="C196" t="s">
+      <c r="C206" t="s">
         <v>394</v>
       </c>
-      <c r="D196" t="s">
+      <c r="D206" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A197" t="s">
-        <v>64</v>
-      </c>
-      <c r="B197" t="str">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A207" t="s">
+        <v>64</v>
+      </c>
+      <c r="B207" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) 인공지능, 머신러닝, 딥러닝 포함 관계 : 머신러닝은 인공지능에 포함, 딥러닝은 머신러닝에 포함 (사용자 질문) 인공지능 머신러닝 딥러닝의 관계는?</v>
       </c>
-      <c r="C197" t="s">
+      <c r="C207" t="s">
         <v>395</v>
       </c>
-      <c r="D197" t="s">
+      <c r="D207" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A198" t="s">
-        <v>64</v>
-      </c>
-      <c r="B198" t="str">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A208" t="s">
+        <v>64</v>
+      </c>
+      <c r="B208" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) 인공지능 정의 : 사람의 인지 능력 (학습, 추론 등) 을 컴퓨터 알고리즘으로 구현하는 기술 (사용자 질문) 인공지능 정의</v>
       </c>
-      <c r="C198" t="s">
+      <c r="C208" t="s">
         <v>396</v>
       </c>
-      <c r="D198" t="s">
+      <c r="D208" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A199" t="s">
-        <v>64</v>
-      </c>
-      <c r="B199" t="str">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A209" t="s">
+        <v>64</v>
+      </c>
+      <c r="B209" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) 머신러닝 정의 : 컴퓨터 알고리즘을 통해, 데이터의 패턴을 학습하여 새로운 데이터에 대해 추론하게 하는 기술 (사용자 질문) 머신러닝은 인공지능에 속하는 거 맞지?</v>
       </c>
-      <c r="C199" t="s">
+      <c r="C209" t="s">
         <v>397</v>
       </c>
-      <c r="D199" t="s">
+      <c r="D209" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A200" t="s">
-        <v>64</v>
-      </c>
-      <c r="B200" t="str">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A210" t="s">
+        <v>64</v>
+      </c>
+      <c r="B210" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) 딥러닝 정의 : 사람의 두뇌를 모방한 인공신경망을 이용한 머신러닝 기술 (사용자 질문) 딥러닝이 뭔지 알려줘</v>
       </c>
-      <c r="C200" t="s">
+      <c r="C210" t="s">
         <v>398</v>
       </c>
-      <c r="D200" t="s">
+      <c r="D210" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A201" t="s">
-        <v>64</v>
-      </c>
-      <c r="B201" t="str">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A211" t="s">
+        <v>64</v>
+      </c>
+      <c r="B211" t="str">
         <f t="shared" si="1"/>
         <v>(제공된 정보) Learning Rate (학습률) : 딥러닝 모델에서 오차 역전파를 하기 위한 미분값 (기울기) 에 곱하는 배수 (사용자 질문) 딥러닝의 learning rate 그게 뭐지?</v>
       </c>
-      <c r="C201" t="s">
+      <c r="C211" t="s">
         <v>399</v>
       </c>
-      <c r="D201" t="s">
+      <c r="D211" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A202" t="s">
-        <v>64</v>
-      </c>
-      <c r="B202" t="str">
-        <f t="shared" ref="B202:B211" si="2">"(제공된 정보) "&amp;D202&amp;" (사용자 질문) "&amp;C202</f>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A212" t="s">
+        <v>64</v>
+      </c>
+      <c r="B212" t="str">
+        <f t="shared" ref="B212:B231" si="2">"(제공된 정보) "&amp;D212&amp;" (사용자 질문) "&amp;C212</f>
         <v>(제공된 정보) Learning Rate (학습률) : 딥러닝 모델에서 오차 역전파를 하기 위한 미분값 (기울기) 에 곱하는 배수 (사용자 질문) 학습률? Learning rate? 뭐야?</v>
       </c>
-      <c r="C202" t="s">
+      <c r="C212" t="s">
         <v>400</v>
       </c>
-      <c r="D202" t="s">
+      <c r="D212" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A203" t="s">
-        <v>64</v>
-      </c>
-      <c r="B203" t="str">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A213" t="s">
+        <v>64</v>
+      </c>
+      <c r="B213" t="str">
         <f t="shared" si="2"/>
         <v>(제공된 정보) Loss Function (손실 함수) 예시 : MSE (Mean-Squared Error), Binary Cross Entropy, Categorical Cross Entropy (사용자 질문) 자주 쓰이는 손실 함수는 뭐가 있을까</v>
       </c>
-      <c r="C203" t="s">
+      <c r="C213" t="s">
         <v>401</v>
       </c>
-      <c r="D203" t="s">
+      <c r="D213" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A204" t="s">
-        <v>64</v>
-      </c>
-      <c r="B204" t="str">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A214" t="s">
+        <v>64</v>
+      </c>
+      <c r="B214" t="str">
         <f t="shared" si="2"/>
         <v>(제공된 정보) Overfitting (과적합) : 딥러닝 모델 학습이 과도하게 train data 에 최적화되어 오히려 성능이 떨어지는 현상 (사용자 질문) 오버피팅이 뭐야</v>
       </c>
-      <c r="C204" t="s">
+      <c r="C214" t="s">
         <v>402</v>
       </c>
-      <c r="D204" t="s">
+      <c r="D214" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A205" t="s">
-        <v>64</v>
-      </c>
-      <c r="B205" t="str">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A215" t="s">
+        <v>64</v>
+      </c>
+      <c r="B215" t="str">
         <f t="shared" si="2"/>
         <v>(제공된 정보) Overfitting (과적합) 해결 방법 : Early Stopping, Cross Validation, Batch Normalization, Dropout 등 (사용자 질문) Overfitting 대체 어떻게 해결하지?</v>
       </c>
-      <c r="C205" t="s">
+      <c r="C215" t="s">
         <v>403</v>
       </c>
-      <c r="D205" t="s">
+      <c r="D215" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A206" t="s">
-        <v>64</v>
-      </c>
-      <c r="B206" t="str">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A216" t="s">
+        <v>64</v>
+      </c>
+      <c r="B216" t="str">
         <f t="shared" si="2"/>
         <v>(제공된 정보) Transfer Learning (전이학습) : 이미 학습된 모델을 다른 문제에 최적화하도록 추가 학습시키는 것 (사용자 질문) 전이학습? 그게 뭐야 도대체?</v>
       </c>
-      <c r="C206" t="s">
+      <c r="C216" t="s">
         <v>404</v>
       </c>
-      <c r="D206" t="s">
+      <c r="D216" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A207" t="s">
-        <v>64</v>
-      </c>
-      <c r="B207" t="str">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A217" t="s">
+        <v>64</v>
+      </c>
+      <c r="B217" t="str">
         <f t="shared" si="2"/>
         <v>(제공된 정보) Transfer Learning (전이학습) : 이미 학습된 모델을 다른 문제에 최적화하도록 추가 학습시키는 것 (사용자 질문) Transfer Learning 요즘 대세라던데 뭐야</v>
       </c>
-      <c r="C207" t="s">
+      <c r="C217" t="s">
         <v>405</v>
       </c>
-      <c r="D207" t="s">
+      <c r="D217" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A208" t="s">
-        <v>64</v>
-      </c>
-      <c r="B208" t="str">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A218" t="s">
+        <v>64</v>
+      </c>
+      <c r="B218" t="str">
         <f t="shared" si="2"/>
         <v>(제공된 정보) Activation Function (활성화 함수) : 딥러닝 신경망의 특정 층에서, 데이터의 총합을 변형하여 다음 층으로 전달하기 위한 함수 (사용자 질문) 활성화 함수? 뭐야?</v>
       </c>
-      <c r="C208" t="s">
+      <c r="C218" t="s">
         <v>406</v>
       </c>
-      <c r="D208" t="s">
+      <c r="D218" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A209" t="s">
-        <v>64</v>
-      </c>
-      <c r="B209" t="str">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A219" t="s">
+        <v>64</v>
+      </c>
+      <c r="B219" t="str">
         <f t="shared" si="2"/>
         <v>(제공된 정보) Activation Function (활성화 함수) 사용 이유 : 비선형의 활성화 함수가 없으면 아무리 학습해도 선형 결합만 학습 가능 (사용자 질문) 굳이 활성화 함수 왜 써?</v>
       </c>
-      <c r="C209" t="s">
+      <c r="C219" t="s">
         <v>407</v>
       </c>
-      <c r="D209" t="s">
+      <c r="D219" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A210" t="s">
-        <v>64</v>
-      </c>
-      <c r="B210" t="str">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A220" t="s">
+        <v>64</v>
+      </c>
+      <c r="B220" t="str">
         <f t="shared" si="2"/>
         <v>(제공된 정보) CNN (합성곱 신경망) : 인간의 시각 지능을 모방한 딥러닝 알고리즘으로, 이미지 인식을 위해 주로 사용 | 핵심 가정 : 이미지에서 이웃한 픽셀의 값이 서로 비슷함 (사용자 질문) CNN이 뭐야? 이미지 인식에 좋다던데</v>
       </c>
-      <c r="C210" t="s">
+      <c r="C220" t="s">
         <v>408</v>
       </c>
-      <c r="D210" t="s">
+      <c r="D220" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A211" t="s">
-        <v>64</v>
-      </c>
-      <c r="B211" t="str">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A221" t="s">
+        <v>64</v>
+      </c>
+      <c r="B221" t="str">
         <f t="shared" si="2"/>
         <v>(제공된 정보) Large Language Model (LLM, 거대 언어 모델) : 텍스트로 주어지는 사용자의 질문에 대해 적절한 답변을 생성하는 생성형 AI 모델 (사용자 질문) LLM이 정확히 뭐야? 나도 AI 트렌드 따라잡자!!</v>
       </c>
-      <c r="C211" t="s">
+      <c r="C221" t="s">
         <v>409</v>
       </c>
-      <c r="D211" t="s">
+      <c r="D221" t="s">
         <v>333</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A222" t="s">
+        <v>64</v>
+      </c>
+      <c r="B222" t="str">
+        <f t="shared" si="2"/>
+        <v>(제공된 정보) 알맞은 정보를 찾을 수 없음 (사용자 질문) Probability 랑 Likelihood 의 차이를 자세히 알려줘</v>
+      </c>
+      <c r="C222" t="s">
+        <v>431</v>
+      </c>
+      <c r="D222" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A223" t="s">
+        <v>64</v>
+      </c>
+      <c r="B223" t="str">
+        <f t="shared" si="2"/>
+        <v>(제공된 정보) 알맞은 정보를 찾을 수 없음 (사용자 질문) tSNE 가 뭐야?</v>
+      </c>
+      <c r="C223" t="s">
+        <v>432</v>
+      </c>
+      <c r="D223" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A224" t="s">
+        <v>64</v>
+      </c>
+      <c r="B224" t="str">
+        <f t="shared" si="2"/>
+        <v>(제공된 정보) 알맞은 정보를 찾을 수 없음 (사용자 질문) 가중치 초기화 중에서 Xavier 가 뭐야</v>
+      </c>
+      <c r="C224" t="s">
+        <v>433</v>
+      </c>
+      <c r="D224" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A225" t="s">
+        <v>64</v>
+      </c>
+      <c r="B225" t="str">
+        <f t="shared" si="2"/>
+        <v>(제공된 정보) 알맞은 정보를 찾을 수 없음 (사용자 질문) AdaGrad 랑 AdaDelta 가 뭔지 알려줘</v>
+      </c>
+      <c r="C225" t="s">
+        <v>434</v>
+      </c>
+      <c r="D225" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A226" t="s">
+        <v>64</v>
+      </c>
+      <c r="B226" t="str">
+        <f t="shared" si="2"/>
+        <v>(제공된 정보) 알맞은 정보를 찾을 수 없음 (사용자 질문) 활성화 함수를 잘못 쓰는 경우는 어떤게 있을까</v>
+      </c>
+      <c r="C226" t="s">
+        <v>435</v>
+      </c>
+      <c r="D226" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A227" t="s">
+        <v>64</v>
+      </c>
+      <c r="B227" t="str">
+        <f t="shared" si="2"/>
+        <v>(제공된 정보) 알맞은 정보를 찾을 수 없음 (사용자 질문) LLM 의 CoT (Chain of Thought) 이 뭔지 궁금해</v>
+      </c>
+      <c r="C227" t="s">
+        <v>436</v>
+      </c>
+      <c r="D227" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A228" t="s">
+        <v>64</v>
+      </c>
+      <c r="B228" t="str">
+        <f t="shared" si="2"/>
+        <v>(제공된 정보) 알맞은 정보를 찾을 수 없음 (사용자 질문) LLM 파인튜닝 중에서 LoRA 가 뭐야?</v>
+      </c>
+      <c r="C228" t="s">
+        <v>437</v>
+      </c>
+      <c r="D228" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A229" t="s">
+        <v>64</v>
+      </c>
+      <c r="B229" t="str">
+        <f t="shared" si="2"/>
+        <v>(제공된 정보) 알맞은 정보를 찾을 수 없음 (사용자 질문) LLM 성능 평가에 자주 쓰이는 벤치마크 데이터셋</v>
+      </c>
+      <c r="C229" t="s">
+        <v>438</v>
+      </c>
+      <c r="D229" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A230" t="s">
+        <v>64</v>
+      </c>
+      <c r="B230" t="str">
+        <f t="shared" si="2"/>
+        <v>(제공된 정보) 알맞은 정보를 찾을 수 없음 (사용자 질문) RAG 가 뭘 목표로 하는지 알려줘</v>
+      </c>
+      <c r="C230" t="s">
+        <v>439</v>
+      </c>
+      <c r="D230" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A231" t="s">
+        <v>64</v>
+      </c>
+      <c r="B231" t="str">
+        <f t="shared" si="2"/>
+        <v>(제공된 정보) 알맞은 정보를 찾을 수 없음 (사용자 질문) 2030년에는 AGI가 나오겠지?</v>
+      </c>
+      <c r="C231" t="s">
+        <v>440</v>
+      </c>
+      <c r="D231" t="s">
+        <v>410</v>
       </c>
     </row>
   </sheetData>

</xml_diff>